<commit_message>
R1 & R2 done
</commit_message>
<xml_diff>
--- a/New-Implementation/Data/sens-data/smaller-full/cw1-cc5-cv10-gam99-smaller-full-nopri-data.xlsx
+++ b/New-Implementation/Data/sens-data/smaller-full/cw1-cc5-cv10-gam99-smaller-full-nopri-data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\Projects\UOttawa-Dynamic-Knapsack-Problem-Python\New-Implementation\Data\sens-data\smaller-full\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\Projects\uOttawa\uOttawa-Dynamic_Knapsack_Problem-Python\New-Implementation\Data\sens-data\smaller-full\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF5BBCDD-7B72-4374-8BAA-8EDC1B8CA057}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9B2260A-F282-496E-A054-95FC10805C25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17340" yWindow="3675" windowWidth="17175" windowHeight="14040" tabRatio="500" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="2010" windowWidth="29040" windowHeight="15840" tabRatio="500" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Indices Data" sheetId="1" r:id="rId1"/>
@@ -1299,7 +1299,7 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1332,7 +1332,7 @@
         <v>27</v>
       </c>
       <c r="I1">
-        <v>0.93</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -1347,7 +1347,7 @@
       </c>
       <c r="D2" s="2">
         <f>I2*$I$1</f>
-        <v>1.2060518731988474</v>
+        <v>1.2319884726224783</v>
       </c>
       <c r="I2" s="2">
         <v>1.2968299711815563</v>
@@ -1369,7 +1369,7 @@
       </c>
       <c r="D3" s="2">
         <f t="shared" ref="D3:D7" si="0">I3*$I$1</f>
-        <v>0.60302593659942372</v>
+        <v>0.61599423631123917</v>
       </c>
       <c r="I3" s="2">
         <v>0.64841498559077815</v>
@@ -1388,7 +1388,7 @@
       </c>
       <c r="D4" s="2">
         <f t="shared" si="0"/>
-        <v>0.14070605187319882</v>
+        <v>0.14373198847262245</v>
       </c>
       <c r="I4" s="2">
         <v>0.15129682997118152</v>
@@ -1407,7 +1407,7 @@
       </c>
       <c r="D5" s="2">
         <f t="shared" si="0"/>
-        <v>0.10050432276657065</v>
+        <v>0.10266570605187322</v>
       </c>
       <c r="I5" s="2">
         <v>0.10806916426512972</v>
@@ -1426,7 +1426,7 @@
       </c>
       <c r="D6" s="2">
         <f t="shared" si="0"/>
-        <v>1.2060518731988474</v>
+        <v>1.2319884726224783</v>
       </c>
       <c r="I6" s="2">
         <v>1.2968299711815563</v>
@@ -1445,7 +1445,7 @@
       </c>
       <c r="D7" s="2">
         <f t="shared" si="0"/>
-        <v>0.60302593659942372</v>
+        <v>0.61599423631123917</v>
       </c>
       <c r="I7" s="2">
         <v>0.64841498559077815</v>

</xml_diff>